<commit_message>
reran questionnaire analysis with corrected questionnaire data
</commit_message>
<xml_diff>
--- a/experiments/2022_scientific_reports/results/statistics/stats_questionnaire_mdbf_interaction.xlsx
+++ b/experiments/2022_scientific_reports/results/statistics/stats_questionnaire_mdbf_interaction.xlsx
@@ -167,34 +167,34 @@
     <t>9.635</t>
   </si>
   <si>
-    <t>0.869</t>
-  </si>
-  <si>
-    <t>0.771</t>
-  </si>
-  <si>
-    <t>0.647</t>
+    <t>0.586</t>
+  </si>
+  <si>
+    <t>0.667</t>
+  </si>
+  <si>
+    <t>0.438</t>
   </si>
   <si>
     <t>1.802e+05</t>
   </si>
   <si>
-    <t>0.392</t>
+    <t>0.467</t>
+  </si>
+  <si>
+    <t>0.615</t>
+  </si>
+  <si>
+    <t>0.368</t>
+  </si>
+  <si>
+    <t>7.884e+05</t>
+  </si>
+  <si>
+    <t>0.495</t>
   </si>
   <si>
     <t>0.369</t>
-  </si>
-  <si>
-    <t>0.505</t>
-  </si>
-  <si>
-    <t>7.884e+05</t>
-  </si>
-  <si>
-    <t>0.376</t>
-  </si>
-  <si>
-    <t>0.373</t>
   </si>
   <si>
     <t>Pairwise Tests</t>
@@ -654,10 +654,10 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>0.9145</v>
+        <v>0.9314</v>
       </c>
       <c r="E3">
-        <v>0.2436</v>
+        <v>0.3953</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -670,10 +670,10 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>0.955</v>
+        <v>0.949</v>
       </c>
       <c r="E4">
-        <v>0.676</v>
+        <v>0.5839</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -688,10 +688,10 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <v>0.9478</v>
+        <v>0.9624</v>
       </c>
       <c r="E5">
-        <v>0.6051</v>
+        <v>0.8173</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -704,10 +704,10 @@
         <v>19</v>
       </c>
       <c r="D6">
-        <v>0.8975</v>
+        <v>0.9</v>
       </c>
       <c r="E6">
-        <v>0.1234</v>
+        <v>0.1339</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>0.9382</v>
+        <v>0.9167999999999999</v>
       </c>
       <c r="E7">
-        <v>0.4755</v>
+        <v>0.2606</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -740,10 +740,10 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>0.9745</v>
+        <v>0.9529</v>
       </c>
       <c r="E8">
-        <v>0.9412</v>
+        <v>0.6433</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>0.824</v>
+        <v>0.8181</v>
       </c>
       <c r="E9">
-        <v>0.0178</v>
+        <v>0.0152</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -774,10 +774,10 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>0.9656</v>
+        <v>0.9473</v>
       </c>
       <c r="E10">
-        <v>0.8362000000000001</v>
+        <v>0.5587</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -794,10 +794,10 @@
         <v>18</v>
       </c>
       <c r="D11">
-        <v>0.9593</v>
+        <v>0.9631</v>
       </c>
       <c r="E11">
-        <v>0.7734</v>
+        <v>0.8267</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -810,10 +810,10 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>0.9194</v>
+        <v>0.8824</v>
       </c>
       <c r="E12">
-        <v>0.2464</v>
+        <v>0.0769</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -828,10 +828,10 @@
         <v>18</v>
       </c>
       <c r="D13">
-        <v>0.9498</v>
+        <v>0.9609</v>
       </c>
       <c r="E13">
-        <v>0.6347</v>
+        <v>0.7959000000000001</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -844,10 +844,10 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>0.9096</v>
+        <v>0.9126</v>
       </c>
       <c r="E14">
-        <v>0.1809</v>
+        <v>0.1987</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -911,10 +911,10 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>0.3335</v>
+        <v>0.2057</v>
       </c>
       <c r="E3">
-        <v>0.5692</v>
+        <v>0.6544</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -929,10 +929,10 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>1.6634</v>
+        <v>2.9337</v>
       </c>
       <c r="E4">
-        <v>0.21</v>
+        <v>0.1002</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -949,10 +949,10 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>0.0203</v>
+        <v>0.6622</v>
       </c>
       <c r="E5">
-        <v>0.8879</v>
+        <v>0.4241</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -967,10 +967,10 @@
         <v>22</v>
       </c>
       <c r="D6">
-        <v>0.7395</v>
+        <v>0.1763</v>
       </c>
       <c r="E6">
-        <v>0.3987</v>
+        <v>0.6785</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -987,10 +987,10 @@
         <v>22</v>
       </c>
       <c r="D7">
-        <v>0.3599</v>
+        <v>1.8029</v>
       </c>
       <c r="E7">
-        <v>0.5544</v>
+        <v>0.1925</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -1005,10 +1005,10 @@
         <v>22</v>
       </c>
       <c r="D8">
-        <v>0.1259</v>
+        <v>0.2494</v>
       </c>
       <c r="E8">
-        <v>0.726</v>
+        <v>0.6222</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1081,7 +1081,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>103.155</v>
+        <v>57.8954</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1090,16 +1090,16 @@
         <v>23</v>
       </c>
       <c r="G3">
-        <v>103.155</v>
+        <v>57.8954</v>
       </c>
       <c r="H3">
-        <v>2.3558</v>
+        <v>1.2653</v>
       </c>
       <c r="I3">
-        <v>0.1385</v>
+        <v>0.2723</v>
       </c>
       <c r="J3">
-        <v>0.0929</v>
+        <v>0.0521</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1123,13 +1123,13 @@
         <v>131.22</v>
       </c>
       <c r="H4">
-        <v>9.5185</v>
+        <v>9.6745</v>
       </c>
       <c r="I4">
-        <v>0.0052</v>
+        <v>0.0049</v>
       </c>
       <c r="J4">
-        <v>0.2927</v>
+        <v>0.2961</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1144,7 +1144,7 @@
         <v>33</v>
       </c>
       <c r="D5">
-        <v>1.2063</v>
+        <v>6.3184</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1153,16 +1153,16 @@
         <v>23</v>
       </c>
       <c r="G5">
-        <v>1.2063</v>
+        <v>6.3184</v>
       </c>
       <c r="H5">
-        <v>0.08749999999999999</v>
+        <v>0.4658</v>
       </c>
       <c r="I5">
-        <v>0.77</v>
+        <v>0.5017</v>
       </c>
       <c r="J5">
-        <v>0.0038</v>
+        <v>0.0199</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1176,7 +1176,7 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>9.8371</v>
+        <v>35.0678</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1185,16 +1185,16 @@
         <v>23</v>
       </c>
       <c r="G6">
-        <v>9.8371</v>
+        <v>35.0678</v>
       </c>
       <c r="H6">
-        <v>0.1762</v>
+        <v>0.6408</v>
       </c>
       <c r="I6">
-        <v>0.6785</v>
+        <v>0.4316</v>
       </c>
       <c r="J6">
-        <v>0.0076</v>
+        <v>0.0271</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1218,13 +1218,13 @@
         <v>1404.5</v>
       </c>
       <c r="H7">
-        <v>56.4902</v>
+        <v>58.1726</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.7107</v>
+        <v>0.7167</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1239,7 +1239,7 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>16.157</v>
+        <v>32.6955</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1248,16 +1248,16 @@
         <v>23</v>
       </c>
       <c r="G8">
-        <v>16.157</v>
+        <v>32.6955</v>
       </c>
       <c r="H8">
-        <v>0.6498</v>
+        <v>1.3542</v>
       </c>
       <c r="I8">
-        <v>0.4284</v>
+        <v>0.2565</v>
       </c>
       <c r="J8">
-        <v>0.0275</v>
+        <v>0.0556</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1271,7 +1271,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>2.3713</v>
+        <v>33.8713</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1280,16 +1280,16 @@
         <v>23</v>
       </c>
       <c r="G9">
-        <v>2.3713</v>
+        <v>33.8713</v>
       </c>
       <c r="H9">
-        <v>0.0538</v>
+        <v>0.7938</v>
       </c>
       <c r="I9">
-        <v>0.8186</v>
+        <v>0.3822</v>
       </c>
       <c r="J9">
-        <v>0.0023</v>
+        <v>0.0334</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1313,13 +1313,13 @@
         <v>2060.82</v>
       </c>
       <c r="H10">
-        <v>65.7966</v>
+        <v>69.539</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.741</v>
+        <v>0.7514999999999999</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1334,7 +1334,7 @@
         <v>33</v>
       </c>
       <c r="D11">
-        <v>0.2954</v>
+        <v>39.0646</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1343,16 +1343,16 @@
         <v>23</v>
       </c>
       <c r="G11">
-        <v>0.2954</v>
+        <v>39.0646</v>
       </c>
       <c r="H11">
-        <v>0.0094</v>
+        <v>1.3182</v>
       </c>
       <c r="I11">
-        <v>0.9235</v>
+        <v>0.2627</v>
       </c>
       <c r="J11">
-        <v>0.0004</v>
+        <v>0.0542</v>
       </c>
     </row>
   </sheetData>
@@ -1488,22 +1488,22 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1.5485</v>
+        <v>1.1317</v>
       </c>
       <c r="J4">
-        <v>22.6175</v>
+        <v>22.9078</v>
       </c>
       <c r="K4" t="s">
         <v>47</v>
       </c>
       <c r="L4">
-        <v>0.1354</v>
+        <v>0.2695</v>
       </c>
       <c r="M4" t="s">
         <v>49</v>
       </c>
       <c r="N4">
-        <v>0.5942</v>
+        <v>0.4355</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1530,22 +1530,22 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1.4334</v>
+        <v>1.282</v>
       </c>
       <c r="J5">
-        <v>21.6593</v>
+        <v>22.2886</v>
       </c>
       <c r="K5" t="s">
         <v>47</v>
       </c>
       <c r="L5">
-        <v>0.166</v>
+        <v>0.213</v>
       </c>
       <c r="M5" t="s">
         <v>50</v>
       </c>
       <c r="N5">
-        <v>0.5588</v>
+        <v>0.4983</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1572,22 +1572,22 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1.2469</v>
+        <v>0.6892</v>
       </c>
       <c r="J6">
-        <v>21.3984</v>
+        <v>20.0744</v>
       </c>
       <c r="K6" t="s">
         <v>47</v>
       </c>
       <c r="L6">
-        <v>0.2259</v>
+        <v>0.4986</v>
       </c>
       <c r="M6" t="s">
         <v>51</v>
       </c>
       <c r="N6">
-        <v>0.4757</v>
+        <v>0.2618</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1658,22 +1658,22 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>-0.4152</v>
+        <v>0.8073</v>
       </c>
       <c r="J8">
-        <v>20.533</v>
+        <v>22.6763</v>
       </c>
       <c r="K8" t="s">
         <v>47</v>
       </c>
       <c r="L8">
-        <v>0.6823</v>
+        <v>0.4279</v>
       </c>
       <c r="M8" t="s">
         <v>53</v>
       </c>
       <c r="N8">
-        <v>-0.1625</v>
+        <v>0.3099</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1700,22 +1700,22 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>0.0868</v>
+        <v>1.1896</v>
       </c>
       <c r="J9">
-        <v>22.969</v>
+        <v>21.9495</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
       </c>
       <c r="L9">
-        <v>0.9316</v>
+        <v>0.2469</v>
       </c>
       <c r="M9" t="s">
         <v>54</v>
       </c>
       <c r="N9">
-        <v>0.0335</v>
+        <v>0.4548</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1742,22 +1742,22 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>-0.9294</v>
+        <v>0.0265</v>
       </c>
       <c r="J10">
-        <v>18.7651</v>
+        <v>22.9998</v>
       </c>
       <c r="K10" t="s">
         <v>47</v>
       </c>
       <c r="L10">
-        <v>0.3645</v>
+        <v>0.9791</v>
       </c>
       <c r="M10" t="s">
         <v>55</v>
       </c>
       <c r="N10">
-        <v>-0.3658</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1828,22 +1828,22 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>-0.2339</v>
+        <v>0.8998</v>
       </c>
       <c r="J12">
-        <v>22.7069</v>
+        <v>22.4616</v>
       </c>
       <c r="K12" t="s">
         <v>47</v>
       </c>
       <c r="L12">
-        <v>0.8171</v>
+        <v>0.3778</v>
       </c>
       <c r="M12" t="s">
         <v>57</v>
       </c>
       <c r="N12">
-        <v>-0.0898</v>
+        <v>0.3449</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1870,22 +1870,22 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>-0.1891</v>
+        <v>1.1317</v>
       </c>
       <c r="J13">
-        <v>22.9381</v>
+        <v>21.9648</v>
       </c>
       <c r="K13" t="s">
         <v>47</v>
       </c>
       <c r="L13">
-        <v>0.8517</v>
+        <v>0.27</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="N13">
-        <v>-0.0728</v>
+        <v>0.4327</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1912,22 +1912,22 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>-0.1884</v>
+        <v>-0.081</v>
       </c>
       <c r="J14">
-        <v>22.8679</v>
+        <v>22.4056</v>
       </c>
       <c r="K14" t="s">
         <v>47</v>
       </c>
       <c r="L14">
-        <v>0.8522</v>
+        <v>0.9361</v>
       </c>
       <c r="M14" t="s">
         <v>58</v>
       </c>
       <c r="N14">
-        <v>-0.07290000000000001</v>
+        <v>-0.0315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>